<commit_message>
added pascal and jacobi-1D vary blocksize experiments
</commit_message>
<xml_diff>
--- a/Journals to Submit to.xlsx
+++ b/Journals to Submit to.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="-60" yWindow="0" windowWidth="24920" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="81">
   <si>
     <t>Possible Journals to Submit to</t>
   </si>
@@ -243,9 +243,6 @@
     <t>Input size</t>
   </si>
   <si>
-    <t>Comparison to Related Work</t>
-  </si>
-  <si>
     <t>Writing Improvements</t>
   </si>
   <si>
@@ -259,6 +256,12 @@
   </si>
   <si>
     <t>If we can do case study thing, do it by Sept 26</t>
+  </si>
+  <si>
+    <t>Varying the block size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantitative Comparison to Related Work - looking for other methods that apply to cyclic or block cyclic </t>
   </si>
 </sst>
 </file>
@@ -271,7 +274,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -673,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G77"/>
+  <dimension ref="A2:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1113,7 +1115,7 @@
         <v>2</v>
       </c>
       <c r="B71" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1121,7 +1123,7 @@
         <v>3</v>
       </c>
       <c r="B72" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1129,22 +1131,30 @@
         <v>4</v>
       </c>
       <c r="B73" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="B75" t="s">
-        <v>77</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74">
+        <v>5</v>
+      </c>
+      <c r="B74" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="B76" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="B77" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="B78" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Journal paper for JPC complete
</commit_message>
<xml_diff>
--- a/Journals to Submit to.xlsx
+++ b/Journals to Submit to.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="0" windowWidth="24920" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="-60" yWindow="0" windowWidth="24900" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="83">
   <si>
     <t>Possible Journals to Submit to</t>
   </si>
@@ -262,6 +262,12 @@
   </si>
   <si>
     <t xml:space="preserve">Quantitative Comparison to Related Work - looking for other methods that apply to cyclic or block cyclic </t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>WORKING ON IT</t>
   </si>
 </sst>
 </file>
@@ -677,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -828,7 +834,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="1:5">
       <c r="B17" t="s">
         <v>32</v>
       </c>
@@ -836,7 +842,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="1:5">
       <c r="B18" t="s">
         <v>33</v>
       </c>
@@ -844,7 +850,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="1:5">
       <c r="B19" t="s">
         <v>29</v>
       </c>
@@ -858,7 +864,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="1:5">
       <c r="B21" t="s">
         <v>34</v>
       </c>
@@ -872,17 +878,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>81</v>
+      </c>
       <c r="B22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="1:5">
       <c r="B23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="1:5">
       <c r="B25" t="s">
         <v>38</v>
       </c>
@@ -896,17 +905,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="1:5">
       <c r="B26" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="1:5">
       <c r="B27" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="2:5">
+    <row r="29" spans="1:5">
       <c r="B29" t="s">
         <v>39</v>
       </c>
@@ -920,27 +929,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:5">
+    <row r="30" spans="1:5">
       <c r="B30" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="2:5">
+    <row r="31" spans="1:5">
       <c r="B31" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="2:5">
+    <row r="32" spans="1:5">
       <c r="B32" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="1:5">
       <c r="B33" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="2:5">
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>81</v>
+      </c>
       <c r="B35" t="s">
         <v>45</v>
       </c>
@@ -954,17 +966,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:5">
+    <row r="36" spans="1:5">
       <c r="B36" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="2:5">
+    <row r="37" spans="1:5">
       <c r="B37" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="2:5">
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>81</v>
+      </c>
       <c r="B39" t="s">
         <v>59</v>
       </c>
@@ -978,22 +993,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="2:5">
+    <row r="40" spans="1:5">
       <c r="B40" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="2:5">
+    <row r="41" spans="1:5">
       <c r="B41" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="2:5">
+    <row r="42" spans="1:5">
       <c r="B42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="2:5">
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>82</v>
+      </c>
       <c r="B44" t="s">
         <v>52</v>
       </c>
@@ -1007,7 +1025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="2:5">
+    <row r="46" spans="1:5">
       <c r="B46" t="s">
         <v>56</v>
       </c>
@@ -1021,32 +1039,38 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="2:5">
+    <row r="47" spans="1:5">
       <c r="B47" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="2:5">
+    <row r="48" spans="1:5">
       <c r="B48" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="2:5">
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>81</v>
+      </c>
       <c r="B50" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="2:5">
+    <row r="52" spans="1:5">
       <c r="B52" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="2:5">
+    <row r="54" spans="1:5">
       <c r="B54" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="2:5">
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>81</v>
+      </c>
       <c r="B56" t="s">
         <v>61</v>
       </c>
@@ -1057,32 +1081,32 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="2:5">
+    <row r="57" spans="1:5">
       <c r="B57" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="2:5">
+    <row r="59" spans="1:5">
       <c r="B59" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="2:5">
+    <row r="60" spans="1:5">
       <c r="B60" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="2:5">
+    <row r="61" spans="1:5">
       <c r="B61" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="2:5">
+    <row r="63" spans="1:5">
       <c r="B63" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="2:5">
+    <row r="64" spans="1:5">
       <c r="B64" t="s">
         <v>68</v>
       </c>

</xml_diff>